<commit_message>
Fix the missing sensor Excel sheet entry 'Leistung' since the FST Label Creator awaits it
</commit_message>
<xml_diff>
--- a/excel_tables/sensor_table.xlsx
+++ b/excel_tables/sensor_table.xlsx
@@ -5,20 +5,22 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Druck" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Kraft" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Weg" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Temperatur" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Volumenstrom" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Leistung" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Volumenstrom" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Druck!$A$1:$AO$2</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Kraft!$A$1:$AM$2</definedName>
+    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Leistung!$A$1:$AQ$2</definedName>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Temperatur!$A$1:$AM$2</definedName>
-    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Volumenstrom!$A$1:$AM$2</definedName>
+    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Volumenstrom!$A$1:$AM$2</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Weg!$A$1:$AM$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="57">
   <si>
     <t xml:space="preserve">uuid</t>
   </si>
@@ -154,18 +156,67 @@
   </si>
   <si>
     <t xml:space="preserve">Datasheet FST-Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensor Messbereich von</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensor Messbereich bis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensor Messbereich Einheit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensor Ausgabebereich von</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensor Ausgabebereich bis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensor Ausgabebereich Einheit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensor Kennlinie _ Sensitivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensor Kennlinie _ Bias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute Bias Uncertainty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute Bias Uncertainty Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute Bias Uncertainty Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute Bias Uncertainty Keywords</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relative Bias Uncertainty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relative Bias Uncertainty Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relative Bias Uncertainty Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relative Bias Uncertainty Keywords</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -201,6 +252,21 @@
       <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -314,7 +380,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -367,12 +433,36 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -501,6 +591,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -508,26 +602,26 @@
   </sheetPr>
   <dimension ref="A1:AO203"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C37" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
       <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="0" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="115.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="105.71"/>
@@ -1102,86 +1196,82 @@
       <c r="W68" s="5"/>
       <c r="AB68" s="1"/>
     </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="1"/>
       <c r="P69" s="1"/>
       <c r="U69" s="1"/>
     </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="1"/>
       <c r="P70" s="1"/>
       <c r="U70" s="1"/>
     </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="1"/>
       <c r="P71" s="1"/>
       <c r="U71" s="1"/>
     </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="1"/>
       <c r="P72" s="1"/>
       <c r="U72" s="1"/>
     </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="1"/>
       <c r="P73" s="1"/>
       <c r="U73" s="1"/>
     </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="1"/>
       <c r="P74" s="1"/>
       <c r="U74" s="1"/>
     </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="1"/>
       <c r="P75" s="1"/>
       <c r="U75" s="1"/>
     </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="1"/>
       <c r="P76" s="1"/>
       <c r="U76" s="6"/>
     </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="1"/>
       <c r="P77" s="1"/>
       <c r="U77" s="6"/>
     </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="1"/>
       <c r="P78" s="1"/>
       <c r="U78" s="6"/>
     </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="1"/>
       <c r="P79" s="1"/>
       <c r="U79" s="1"/>
     </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="1"/>
       <c r="P80" s="1"/>
       <c r="U80" s="1"/>
     </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="1"/>
       <c r="P81" s="1"/>
       <c r="U81" s="1"/>
     </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="1"/>
       <c r="P82" s="1"/>
       <c r="U82" s="1"/>
     </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="1"/>
       <c r="P83" s="1"/>
       <c r="U83" s="1"/>
     </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="1"/>
       <c r="P88" s="1"/>
       <c r="U88" s="1"/>
@@ -1190,7 +1280,7 @@
       <c r="AB88" s="7"/>
       <c r="AC88" s="8"/>
     </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="1"/>
       <c r="P89" s="1"/>
       <c r="U89" s="1"/>
@@ -1199,7 +1289,7 @@
       <c r="AB89" s="7"/>
       <c r="AC89" s="8"/>
     </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="1"/>
       <c r="P90" s="1"/>
       <c r="U90" s="1"/>
@@ -1208,7 +1298,7 @@
       <c r="AB90" s="7"/>
       <c r="AC90" s="8"/>
     </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="1"/>
       <c r="P91" s="1"/>
       <c r="U91" s="1"/>
@@ -1217,7 +1307,7 @@
       <c r="AB91" s="7"/>
       <c r="AC91" s="8"/>
     </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="1"/>
       <c r="P92" s="1"/>
       <c r="U92" s="1"/>
@@ -1226,31 +1316,6 @@
       <c r="AB92" s="7"/>
       <c r="AC92" s="8"/>
     </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P135" s="1"/>
     </row>
@@ -1519,25 +1584,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AM35"/>
+  <dimension ref="A1:AM68"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AD3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="AD1" activeCellId="0" sqref="AD1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
       <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="20.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.71"/>
@@ -1548,7 +1613,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="16.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="16.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="14.15"/>
   </cols>
   <sheetData>
@@ -1773,78 +1838,111 @@
       <c r="Z13" s="5"/>
       <c r="AE13" s="1"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="1"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="1"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="1"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="1"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="1"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="1"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="1"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="1"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="1"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="1"/>
     </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A1:AM2"/>
   <mergeCells count="39">
@@ -1907,26 +2005,26 @@
   <dimension ref="A1:AM35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AD3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="AD1" activeCellId="0" sqref="AD1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
       <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="22.86"/>
@@ -2135,9 +2233,6 @@
       <c r="B11" s="1"/>
       <c r="AA11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1"/>
       <c r="P15" s="1"/>
@@ -2277,26 +2372,26 @@
   </sheetPr>
   <dimension ref="A1:AM35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="AD3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="AD1" activeCellId="0" sqref="AD1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F37" activeCellId="0" sqref="F37"/>
+      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="65.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="21.14"/>
@@ -2305,10 +2400,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="42.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="0" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="0" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="18.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="19.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="15.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="15.87"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2748,19 +2843,341 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:AQ4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="25.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="25.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="25.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="24.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="22.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="25.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="23.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="19.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="23.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="28.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="22.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="0" width="22.23"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="S1" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="T1" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="U1" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="V1" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="W1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y1" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z1" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA1" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB1" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC1" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD1" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE1" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF1" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG1" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH1" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI1" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ1" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK1" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL1" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AM1" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO1" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="AP1" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="AQ1" s="16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="18"/>
+      <c r="AC2" s="18"/>
+      <c r="AD2" s="18"/>
+      <c r="AE2" s="16"/>
+      <c r="AF2" s="16"/>
+      <c r="AG2" s="18"/>
+      <c r="AH2" s="16"/>
+      <c r="AI2" s="16"/>
+      <c r="AJ2" s="16"/>
+      <c r="AK2" s="16"/>
+      <c r="AL2" s="16"/>
+      <c r="AM2" s="16"/>
+      <c r="AN2" s="16"/>
+      <c r="AO2" s="16"/>
+      <c r="AP2" s="16"/>
+      <c r="AQ2" s="16"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AI3" s="19"/>
+      <c r="AL3" s="20"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+      <c r="AI4" s="19"/>
+      <c r="AL4" s="20"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:AQ2"/>
+  <mergeCells count="43">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="AC1:AC2"/>
+    <mergeCell ref="AD1:AD2"/>
+    <mergeCell ref="AE1:AE2"/>
+    <mergeCell ref="AF1:AF2"/>
+    <mergeCell ref="AG1:AG2"/>
+    <mergeCell ref="AH1:AH2"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="AJ1:AJ2"/>
+    <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="AM1:AM2"/>
+    <mergeCell ref="AN1:AN2"/>
+    <mergeCell ref="AO1:AO2"/>
+    <mergeCell ref="AP1:AP2"/>
+    <mergeCell ref="AQ1:AQ2"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AM2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.61"/>
@@ -2771,8 +3188,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="19.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="21.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="0" width="22.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="0" width="22.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="25" style="0" width="22.92"/>
   </cols>

</xml_diff>